<commit_message>
First stage in QC sprint 1
</commit_message>
<xml_diff>
--- a/DSmartQB.WEB/Template/Student.xlsx
+++ b/DSmartQB.WEB/Template/Student.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,21 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Firstname</t>
   </si>
   <si>
     <t>Lastname</t>
-  </si>
-  <si>
-    <t>Datebirth</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Nationaid</t>
   </si>
   <si>
     <t>Email</t>
@@ -120,19 +111,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -415,26 +400,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" customWidth="1"/>
-    <col min="5" max="5" width="28" customWidth="1"/>
-    <col min="6" max="6" width="34.42578125" customWidth="1"/>
-    <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" customWidth="1"/>
-    <col min="9" max="9" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
+    <col min="3" max="3" width="34.44140625" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" customWidth="1"/>
+    <col min="6" max="6" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,125 +435,86 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
+      <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
+      <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
+      <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
+      <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
+      <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
+      <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
+      <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
-      <c r="C10" s="3"/>
+      <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>